<commit_message>
BWTracker v0 updated completed !
</commit_message>
<xml_diff>
--- a/BWTracker-v0.xlsx
+++ b/BWTracker-v0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="BWTracker" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>day</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>IoTProject</t>
+  </si>
+  <si>
+    <t>iotMonitor4uhv2n4</t>
+  </si>
+  <si>
+    <t>cfdInvestigation</t>
+  </si>
+  <si>
+    <t>FanReplica</t>
+  </si>
+  <si>
+    <t>MultidimentionalVisualization</t>
   </si>
 </sst>
 </file>
@@ -167,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -178,19 +190,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -510,10 +513,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:EL5"/>
+  <dimension ref="A1:EL2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +530,7 @@
     <col min="11" max="11" width="13" style="2" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="21.5703125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="45.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="45.7109375" style="5" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -565,7 +568,7 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -959,17 +962,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:142" s="4" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="L2" s="6"/>
-      <c r="N2" s="8"/>
-    </row>
-    <row r="3" spans="1:142" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="L3" s="6"/>
-      <c r="N3" s="7"/>
-    </row>
-    <row r="5" spans="1:142" x14ac:dyDescent="0.25">
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+    <row r="2" spans="1:142" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -980,69 +975,98 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42" style="12" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="42" style="9" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="9"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>